<commit_message>
update on property name and coverage status
update on property name and coverage status for M-Extension
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/FormalVerificationPlan/base_instruction_set/CV32E40P_RV32M_Extension_Instructions.xlsx
+++ b/verif/CV32E40P/FormalVerificationPlan/base_instruction_set/CV32E40P_RV32M_Extension_Instructions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntusinschi\Dropbox\OpenHW-Project\forkHW\core-v-docs\verif\CV32E40P\FormalVerificationPlan\base_instruction_set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Dropbox\openHW\core-v-docs\verif\CV32E40P\FormalVerificationPlan\base_instruction_set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C454424A-EAA0-48D0-A864-CE745393432F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E690D128-5ED9-4981-9E64-E73D53CFCFAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -534,18 +534,14 @@
     <t>N/A</t>
   </si>
   <si>
-    <t xml:space="preserve">Each operand is controlled by a parameter defining the number of bits to be tied to '0 or '1:
-(opA[XLEN-1:PARAM]='0 || opA[XLEN-1:PARAM]='1) &amp;&amp; (opB[XLEN-1:PARAM]='0 || opB[XLEN-1:PARAM]='1) </t>
-  </si>
-  <si>
-    <t>Each operand is controlled by a parameter defining the number of bits to be tied to '0 or '1 (default is 1)</t>
+    <t>Regression run with 4 most significant bits and 4 least siginificant bits of either operands free and the remaining bits all set to the same value - all 0 or all 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -605,6 +601,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="DejaVu Sans"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -632,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -665,6 +667,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1082,7 +1087,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="66" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1092,7 +1097,7 @@
     <col min="3" max="3" width="15.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="50.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.5546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -2150,11 +2155,11 @@
       <c r="AMJ1"/>
       <c r="AMK1"/>
     </row>
-    <row r="2" spans="1:1025" ht="55.2">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:1025" ht="42">
+      <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2178,7 +2183,7 @@
       <c r="I2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="13" t="s">
         <v>57</v>
       </c>
       <c r="K2" s="8" t="s">
@@ -2186,8 +2191,8 @@
       </c>
     </row>
     <row r="3" spans="1:1025" s="10" customFormat="1" ht="44.4">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2209,16 +2214,16 @@
       <c r="I3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>58</v>
+      <c r="J3" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:1025" ht="42">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2240,16 +2245,16 @@
       <c r="I4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>58</v>
+      <c r="J4" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:1025" ht="66.599999999999994" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
@@ -2271,18 +2276,18 @@
       <c r="I5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>58</v>
+      <c r="J5" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:1025" ht="66.599999999999994" customHeight="1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2306,16 +2311,16 @@
       <c r="I6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>58</v>
+      <c r="J6" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:1025" ht="69.599999999999994">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
@@ -2326,7 +2331,7 @@
         <v>36</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>33</v>
@@ -2337,16 +2342,16 @@
       <c r="I7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>58</v>
+      <c r="J7" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:1025" ht="67.8" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
+    <row r="8" spans="1:1025" ht="55.8">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
@@ -2357,7 +2362,7 @@
         <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>33</v>
@@ -2368,16 +2373,16 @@
       <c r="I8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>58</v>
+      <c r="J8" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:1025" ht="73.2" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
+    <row r="9" spans="1:1025" ht="56.4">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
@@ -2388,7 +2393,7 @@
         <v>36</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>33</v>
@@ -2399,27 +2404,27 @@
       <c r="I9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>58</v>
+      <c r="J9" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:1025">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:1025">
       <c r="F11" s="5"/>

</xml_diff>